<commit_message>
first commit of catching errors update
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -472,7 +472,7 @@
     <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>5,2726</t>
+          <t>5,3572</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
@@ -494,21 +494,21 @@
     <row r="2" ht="12.8" customHeight="1" s="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>4,3076</t>
+          <t>4,4004</t>
         </is>
       </c>
     </row>
     <row r="3" ht="12.8" customHeight="1" s="2">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>4,5838</t>
+          <t>4,6363</t>
         </is>
       </c>
     </row>
     <row r="4" ht="12.8" customHeight="1" s="2">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>1924,2</t>
+          <t>1874,8</t>
         </is>
       </c>
     </row>
@@ -529,28 +529,28 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>23,54</t>
+          <t>22,5</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>26053,94</t>
+          <t>26438,67</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>0,000688</t>
+          <t>0,000687</t>
         </is>
       </c>
     </row>
     <row r="10" ht="12.8" customHeight="1" s="2">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>1570,81</t>
+          <t>1567,04</t>
         </is>
       </c>
     </row>
@@ -564,21 +564,21 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>0,1424</t>
+          <t>0,1421</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>143,84</t>
+          <t>143,76</t>
         </is>
       </c>
     </row>
     <row r="34" ht="12.8" customHeight="1" s="2">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>60,81</t>
+          <t>6662,0</t>
         </is>
       </c>
     </row>
@@ -642,7 +642,7 @@
     <row r="1" ht="15" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>gbp</t>
+          <t>swda-etf</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
@@ -652,7 +652,7 @@
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>eur</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
@@ -672,7 +672,7 @@
       </c>
       <c r="G1" s="3" t="inlineStr">
         <is>
-          <t>silver</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H1" s="3" t="inlineStr">
@@ -682,27 +682,27 @@
       </c>
       <c r="I1" s="3" t="inlineStr">
         <is>
-          <t>everdome</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J1" s="3" t="inlineStr">
         <is>
-          <t>ethereum</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K1" s="3" t="inlineStr">
         <is>
-          <t>thorchain</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L1" s="3" t="inlineStr">
         <is>
-          <t>mover</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M1" s="3" t="inlineStr">
         <is>
-          <t>monero</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -717,11 +717,7 @@
           <t>Sheet1</t>
         </is>
       </c>
-      <c r="C2" s="3" t="inlineStr">
-        <is>
-          <t>Sheet1</t>
-        </is>
-      </c>
+      <c r="C2" s="3" t="inlineStr"/>
       <c r="D2" s="3" t="inlineStr">
         <is>
           <t>Sheet1</t>
@@ -729,46 +725,22 @@
       </c>
       <c r="E2" s="3" t="inlineStr"/>
       <c r="F2" s="3" t="inlineStr"/>
-      <c r="G2" s="3" t="inlineStr">
+      <c r="G2" s="3" t="inlineStr"/>
+      <c r="H2" s="3" t="inlineStr">
         <is>
           <t>Sheet1</t>
         </is>
       </c>
-      <c r="H2" s="3" t="inlineStr">
-        <is>
-          <t>Sheet1</t>
-        </is>
-      </c>
-      <c r="I2" s="3" t="inlineStr">
-        <is>
-          <t>Sheet1</t>
-        </is>
-      </c>
-      <c r="J2" s="3" t="inlineStr">
-        <is>
-          <t>Sheet1</t>
-        </is>
-      </c>
-      <c r="K2" s="3" t="inlineStr">
-        <is>
-          <t>Sheet1</t>
-        </is>
-      </c>
-      <c r="L2" s="3" t="inlineStr">
-        <is>
-          <t>Sheet1</t>
-        </is>
-      </c>
-      <c r="M2" s="3" t="inlineStr">
-        <is>
-          <t>Sheet1</t>
-        </is>
-      </c>
+      <c r="I2" s="3" t="inlineStr"/>
+      <c r="J2" s="3" t="inlineStr"/>
+      <c r="K2" s="3" t="inlineStr"/>
+      <c r="L2" s="3" t="inlineStr"/>
+      <c r="M2" s="3" t="inlineStr"/>
     </row>
     <row r="3" ht="15" customHeight="1" s="2">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>A1</t>
+          <t>A34</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -776,11 +748,7 @@
           <t>A2</t>
         </is>
       </c>
-      <c r="C3" s="3" t="inlineStr">
-        <is>
-          <t>A3</t>
-        </is>
-      </c>
+      <c r="C3" s="3" t="inlineStr"/>
       <c r="D3" s="3" t="inlineStr">
         <is>
           <t>A4</t>
@@ -788,56 +756,32 @@
       </c>
       <c r="E3" s="3" t="inlineStr"/>
       <c r="F3" s="3" t="inlineStr"/>
-      <c r="G3" s="3" t="inlineStr">
-        <is>
-          <t>A7</t>
-        </is>
-      </c>
+      <c r="G3" s="3" t="inlineStr"/>
       <c r="H3" s="3" t="inlineStr">
         <is>
           <t>A8</t>
         </is>
       </c>
-      <c r="I3" s="3" t="inlineStr">
-        <is>
-          <t>A9</t>
-        </is>
-      </c>
-      <c r="J3" s="3" t="inlineStr">
-        <is>
-          <t>A10</t>
-        </is>
-      </c>
-      <c r="K3" s="3" t="inlineStr">
-        <is>
-          <t>A11</t>
-        </is>
-      </c>
-      <c r="L3" s="3" t="inlineStr">
-        <is>
-          <t>A12</t>
-        </is>
-      </c>
-      <c r="M3" s="3" t="inlineStr">
-        <is>
-          <t>A13</t>
-        </is>
-      </c>
+      <c r="I3" s="3" t="inlineStr"/>
+      <c r="J3" s="3" t="inlineStr"/>
+      <c r="K3" s="3" t="inlineStr"/>
+      <c r="L3" s="3" t="inlineStr"/>
+      <c r="M3" s="3" t="inlineStr"/>
     </row>
     <row r="4" ht="12.8" customHeight="1" s="2">
       <c r="A4" s="3" t="inlineStr">
         <is>
+          <t>GBP</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
           <t>PLN</t>
         </is>
       </c>
-      <c r="B4" s="3" t="inlineStr">
-        <is>
-          <t>PLN</t>
-        </is>
-      </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>PLN</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">

</xml_diff>

<commit_message>
fetch error msg added, colouring buttons with fetch error
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -494,7 +494,7 @@
     <row r="2" ht="12.8" customHeight="1" s="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>4,4004</t>
+          <t>4,404</t>
         </is>
       </c>
     </row>
@@ -508,7 +508,7 @@
     <row r="4" ht="12.8" customHeight="1" s="2">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>1874,8</t>
+          <t>1874,3</t>
         </is>
       </c>
     </row>
@@ -536,7 +536,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>26438,67</t>
+          <t>26408,37</t>
         </is>
       </c>
     </row>
@@ -578,7 +578,7 @@
     <row r="34" ht="12.8" customHeight="1" s="2">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>6662,0</t>
+          <t>6651,0</t>
         </is>
       </c>
     </row>
@@ -642,7 +642,7 @@
     <row r="1" ht="15" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>swda-etf</t>
+          <t>-</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
@@ -707,11 +707,7 @@
       </c>
     </row>
     <row r="2" ht="12.8" customHeight="1" s="2">
-      <c r="A2" s="3" t="inlineStr">
-        <is>
-          <t>Sheet1</t>
-        </is>
-      </c>
+      <c r="A2" s="3" t="inlineStr"/>
       <c r="B2" s="3" t="inlineStr">
         <is>
           <t>Sheet1</t>
@@ -738,11 +734,7 @@
       <c r="M2" s="3" t="inlineStr"/>
     </row>
     <row r="3" ht="15" customHeight="1" s="2">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>A34</t>
-        </is>
-      </c>
+      <c r="A3" s="3" t="inlineStr"/>
       <c r="B3" s="3" t="inlineStr">
         <is>
           <t>A2</t>

</xml_diff>

<commit_message>
textinput modified, colours upgrade
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -461,13 +461,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D213"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G22" activeCellId="1" sqref="A1:A5 G22"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
@@ -494,7 +494,7 @@
     <row r="2" ht="12.8" customHeight="1" s="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>4,404</t>
+          <t>4,36</t>
         </is>
       </c>
     </row>
@@ -508,7 +508,7 @@
     <row r="4" ht="12.8" customHeight="1" s="2">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>1874,3</t>
+          <t>1864,1</t>
         </is>
       </c>
     </row>
@@ -519,28 +519,28 @@
         </is>
       </c>
     </row>
-    <row r="6">
+    <row r="6" ht="12.8" customHeight="1" s="2">
       <c r="A6" s="3" t="inlineStr">
         <is>
           <t>2417,0</t>
         </is>
       </c>
     </row>
-    <row r="7">
+    <row r="7" ht="12.8" customHeight="1" s="2">
       <c r="A7" s="3" t="inlineStr">
         <is>
           <t>22,5</t>
         </is>
       </c>
     </row>
-    <row r="8">
+    <row r="8" ht="12.8" customHeight="1" s="2">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>26408,37</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
+          <t>26982,67</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="12.8" customHeight="1" s="2">
       <c r="A9" s="3" t="inlineStr">
         <is>
           <t>0,000687</t>
@@ -554,21 +554,21 @@
         </is>
       </c>
     </row>
-    <row r="11">
+    <row r="11" ht="12.8" customHeight="1" s="2">
       <c r="A11" s="3" t="inlineStr">
         <is>
           <t>1,7</t>
         </is>
       </c>
     </row>
-    <row r="12">
+    <row r="12" ht="12.8" customHeight="1" s="2">
       <c r="A12" s="3" t="inlineStr">
         <is>
           <t>0,1421</t>
         </is>
       </c>
     </row>
-    <row r="13">
+    <row r="13" ht="12.8" customHeight="1" s="2">
       <c r="A13" s="3" t="inlineStr">
         <is>
           <t>143,76</t>
@@ -579,6 +579,20 @@
       <c r="A34" s="3" t="inlineStr">
         <is>
           <t>6651,0</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="3" t="inlineStr">
+        <is>
+          <t>1680,68</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" s="3" t="inlineStr">
+        <is>
+          <t>27142,11</t>
         </is>
       </c>
     </row>
@@ -606,10 +620,10 @@
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:A5"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData/>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -633,53 +647,53 @@
   </sheetPr>
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:A5"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.82421875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.83984375" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="15" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
+          <t>bitcoin</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>usd</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>ethereum</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
           <t>-</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>usd</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
-        <is>
-          <t>gold</t>
-        </is>
-      </c>
-      <c r="E1" s="3" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="F1" s="3" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="G1" s="3" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="H1" s="3" t="inlineStr">
-        <is>
-          <t>bitcoin</t>
-        </is>
-      </c>
       <c r="I1" s="3" t="inlineStr">
         <is>
           <t>-</t>
@@ -707,63 +721,63 @@
       </c>
     </row>
     <row r="2" ht="12.8" customHeight="1" s="2">
-      <c r="A2" s="3" t="inlineStr"/>
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>Sheet1</t>
+        </is>
+      </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
           <t>Sheet1</t>
         </is>
       </c>
-      <c r="C2" s="3" t="inlineStr"/>
-      <c r="D2" s="3" t="inlineStr">
+      <c r="C2" s="3" t="inlineStr">
         <is>
           <t>Sheet1</t>
         </is>
       </c>
-      <c r="E2" s="3" t="inlineStr"/>
-      <c r="F2" s="3" t="inlineStr"/>
-      <c r="G2" s="3" t="inlineStr"/>
-      <c r="H2" s="3" t="inlineStr">
-        <is>
-          <t>Sheet1</t>
-        </is>
-      </c>
-      <c r="I2" s="3" t="inlineStr"/>
-      <c r="J2" s="3" t="inlineStr"/>
-      <c r="K2" s="3" t="inlineStr"/>
-      <c r="L2" s="3" t="inlineStr"/>
-      <c r="M2" s="3" t="inlineStr"/>
+      <c r="D2" s="3" t="inlineStr"/>
+      <c r="E2" s="3" t="n"/>
+      <c r="F2" s="3" t="n"/>
+      <c r="G2" s="3" t="n"/>
+      <c r="H2" s="3" t="n"/>
+      <c r="I2" s="3" t="n"/>
+      <c r="J2" s="3" t="n"/>
+      <c r="K2" s="3" t="n"/>
+      <c r="L2" s="3" t="n"/>
+      <c r="M2" s="3" t="n"/>
     </row>
     <row r="3" ht="15" customHeight="1" s="2">
-      <c r="A3" s="3" t="inlineStr"/>
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>A213</t>
+        </is>
+      </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
           <t>A2</t>
         </is>
       </c>
-      <c r="C3" s="3" t="inlineStr"/>
-      <c r="D3" s="3" t="inlineStr">
-        <is>
-          <t>A4</t>
-        </is>
-      </c>
-      <c r="E3" s="3" t="inlineStr"/>
-      <c r="F3" s="3" t="inlineStr"/>
-      <c r="G3" s="3" t="inlineStr"/>
-      <c r="H3" s="3" t="inlineStr">
-        <is>
-          <t>A8</t>
-        </is>
-      </c>
-      <c r="I3" s="3" t="inlineStr"/>
-      <c r="J3" s="3" t="inlineStr"/>
-      <c r="K3" s="3" t="inlineStr"/>
-      <c r="L3" s="3" t="inlineStr"/>
-      <c r="M3" s="3" t="inlineStr"/>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>A43</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr"/>
+      <c r="E3" s="3" t="n"/>
+      <c r="F3" s="3" t="n"/>
+      <c r="G3" s="3" t="n"/>
+      <c r="H3" s="3" t="n"/>
+      <c r="I3" s="3" t="n"/>
+      <c r="J3" s="3" t="n"/>
+      <c r="K3" s="3" t="n"/>
+      <c r="L3" s="3" t="n"/>
+      <c r="M3" s="3" t="n"/>
     </row>
     <row r="4" ht="12.8" customHeight="1" s="2">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>GBP</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -858,10 +872,10 @@
   <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A1:A5"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
@@ -929,10 +943,10 @@
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:A5"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData/>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -957,10 +971,10 @@
   <dimension ref="A4:A6"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:A5"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="4" ht="12.8" customHeight="1" s="2">
       <c r="A4" s="3" t="inlineStr">
@@ -1007,10 +1021,10 @@
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:A5"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
@@ -1043,10 +1057,10 @@
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:A5"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData/>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1071,10 +1085,10 @@
   <dimension ref="A45:A45"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:A5"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="45" ht="12.8" customHeight="1" s="2">
       <c r="A45" s="3" t="inlineStr">
@@ -1107,10 +1121,10 @@
   <dimension ref="A3:A4"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:A5"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="3" ht="12.8" customHeight="1" s="2">
       <c r="A3" s="3" t="inlineStr">

</xml_diff>

<commit_message>
update new classes ButtonC and TextInputC
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -472,7 +472,7 @@
     <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>5,3572</t>
+          <t>9,19</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
@@ -494,7 +494,7 @@
     <row r="2" ht="12.8" customHeight="1" s="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>4,36</t>
+          <t>4,3748</t>
         </is>
       </c>
     </row>
@@ -585,14 +585,14 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>1680,68</t>
+          <t>1672,69</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="3" t="inlineStr">
         <is>
-          <t>27142,11</t>
+          <t>26937,03</t>
         </is>
       </c>
     </row>
@@ -656,17 +656,17 @@
     <row r="1" ht="15" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>bitcoin</t>
+          <t>avalanche</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>usd</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>ethereum</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
@@ -726,16 +726,8 @@
           <t>Sheet1</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr">
-        <is>
-          <t>Sheet1</t>
-        </is>
-      </c>
-      <c r="C2" s="3" t="inlineStr">
-        <is>
-          <t>Sheet1</t>
-        </is>
-      </c>
+      <c r="B2" s="3" t="inlineStr"/>
+      <c r="C2" s="3" t="inlineStr"/>
       <c r="D2" s="3" t="inlineStr"/>
       <c r="E2" s="3" t="n"/>
       <c r="F2" s="3" t="n"/>
@@ -750,19 +742,11 @@
     <row r="3" ht="15" customHeight="1" s="2">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>A213</t>
-        </is>
-      </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>A2</t>
-        </is>
-      </c>
-      <c r="C3" s="3" t="inlineStr">
-        <is>
-          <t>A43</t>
-        </is>
-      </c>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr"/>
+      <c r="C3" s="3" t="inlineStr"/>
       <c r="D3" s="3" t="inlineStr"/>
       <c r="E3" s="3" t="n"/>
       <c r="F3" s="3" t="n"/>

</xml_diff>

<commit_message>
ui designing first commit
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -472,7 +472,7 @@
     <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>9,19</t>
+          <t>9,2</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
@@ -645,7 +645,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
@@ -761,12 +761,12 @@
     <row r="4" ht="12.8" customHeight="1" s="2">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>PLN</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>PLN</t>
+          <t>EUR</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">

</xml_diff>

<commit_message>
ui masterpiece version 1.3b Stable
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -472,7 +472,7 @@
     <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>9,2</t>
+          <t>27179,2</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
@@ -645,7 +645,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
@@ -656,7 +656,7 @@
     <row r="1" ht="15" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>avalanche</t>
+          <t>-</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
@@ -721,11 +721,7 @@
       </c>
     </row>
     <row r="2" ht="12.8" customHeight="1" s="2">
-      <c r="A2" s="3" t="inlineStr">
-        <is>
-          <t>Sheet1</t>
-        </is>
-      </c>
+      <c r="A2" s="3" t="inlineStr"/>
       <c r="B2" s="3" t="inlineStr"/>
       <c r="C2" s="3" t="inlineStr"/>
       <c r="D2" s="3" t="inlineStr"/>
@@ -740,11 +736,7 @@
       <c r="M2" s="3" t="n"/>
     </row>
     <row r="3" ht="15" customHeight="1" s="2">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>A1</t>
-        </is>
-      </c>
+      <c r="A3" s="3" t="inlineStr"/>
       <c r="B3" s="3" t="inlineStr"/>
       <c r="C3" s="3" t="inlineStr"/>
       <c r="D3" s="3" t="inlineStr"/>
@@ -761,7 +753,7 @@
     <row r="4" ht="12.8" customHeight="1" s="2">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>PLN</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">

</xml_diff>

<commit_message>
add button improved, background logo added and some small changes in ui
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -492,7 +492,7 @@
       </c>
       <c r="S1" s="3" t="inlineStr">
         <is>
-          <t>28088,09</t>
+          <t>28334,01</t>
         </is>
       </c>
     </row>
@@ -650,7 +650,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>

</xml_diff>

<commit_message>
added asset logo (only crypto for now)
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -673,7 +673,7 @@
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ethereum</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
@@ -683,22 +683,22 @@
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>usd</t>
         </is>
       </c>
       <c r="E1" s="3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>emim-etf</t>
         </is>
       </c>
       <c r="F1" s="3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>gold</t>
         </is>
       </c>
       <c r="G1" s="3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>litecoin</t>
         </is>
       </c>
       <c r="H1" s="3" t="inlineStr">
@@ -738,16 +738,36 @@
           <t>Sheet1</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr"/>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>Arkusz3</t>
+        </is>
+      </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
           <t>Arkusz3</t>
         </is>
       </c>
-      <c r="D2" s="3" t="inlineStr"/>
-      <c r="E2" s="3" t="n"/>
-      <c r="F2" s="3" t="n"/>
-      <c r="G2" s="3" t="n"/>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>Arkusz3</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="inlineStr">
+        <is>
+          <t>Sheet1</t>
+        </is>
+      </c>
+      <c r="F2" s="3" t="inlineStr">
+        <is>
+          <t>Arkusz3</t>
+        </is>
+      </c>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>Arkusz3</t>
+        </is>
+      </c>
       <c r="H2" s="3" t="n"/>
       <c r="I2" s="3" t="n"/>
       <c r="J2" s="3" t="n"/>
@@ -761,16 +781,36 @@
           <t>A1</t>
         </is>
       </c>
-      <c r="B3" s="3" t="inlineStr"/>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>A45</t>
+        </is>
+      </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
           <t>A5</t>
         </is>
       </c>
-      <c r="D3" s="3" t="inlineStr"/>
-      <c r="E3" s="3" t="n"/>
-      <c r="F3" s="3" t="n"/>
-      <c r="G3" s="3" t="n"/>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>A45</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="inlineStr">
+        <is>
+          <t>A23</t>
+        </is>
+      </c>
+      <c r="F3" s="3" t="inlineStr">
+        <is>
+          <t>A56</t>
+        </is>
+      </c>
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t>A234</t>
+        </is>
+      </c>
       <c r="H3" s="3" t="n"/>
       <c r="I3" s="3" t="n"/>
       <c r="J3" s="3" t="n"/>
@@ -786,27 +826,27 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
           <t>USD</t>
         </is>
       </c>
-      <c r="C4" s="3" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
-      <c r="D4" s="3" t="inlineStr">
+      <c r="F4" s="3" t="inlineStr">
         <is>
           <t>USD</t>
-        </is>
-      </c>
-      <c r="E4" s="3" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
-      <c r="F4" s="3" t="inlineStr">
-        <is>
-          <t>GBP</t>
         </is>
       </c>
       <c r="G4" s="3" t="inlineStr">

</xml_diff>

<commit_message>
added logos for ishares gold silver usd gbp eur
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -673,32 +673,32 @@
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>ethereum</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>amp</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
         <is>
-          <t>usd</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E1" s="3" t="inlineStr">
         <is>
-          <t>emim-etf</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F1" s="3" t="inlineStr">
         <is>
-          <t>gold</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G1" s="3" t="inlineStr">
         <is>
-          <t>litecoin</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H1" s="3" t="inlineStr">
@@ -738,39 +738,15 @@
           <t>Sheet1</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr">
-        <is>
-          <t>Arkusz3</t>
-        </is>
-      </c>
-      <c r="C2" s="3" t="inlineStr">
-        <is>
-          <t>Arkusz3</t>
-        </is>
-      </c>
-      <c r="D2" s="3" t="inlineStr">
-        <is>
-          <t>Arkusz3</t>
-        </is>
-      </c>
-      <c r="E2" s="3" t="inlineStr">
-        <is>
-          <t>Sheet1</t>
-        </is>
-      </c>
-      <c r="F2" s="3" t="inlineStr">
-        <is>
-          <t>Arkusz3</t>
-        </is>
-      </c>
-      <c r="G2" s="3" t="inlineStr">
-        <is>
-          <t>Arkusz3</t>
-        </is>
-      </c>
-      <c r="H2" s="3" t="n"/>
-      <c r="I2" s="3" t="n"/>
-      <c r="J2" s="3" t="n"/>
+      <c r="B2" s="3" t="inlineStr"/>
+      <c r="C2" s="3" t="inlineStr"/>
+      <c r="D2" s="3" t="inlineStr"/>
+      <c r="E2" s="3" t="inlineStr"/>
+      <c r="F2" s="3" t="inlineStr"/>
+      <c r="G2" s="3" t="inlineStr"/>
+      <c r="H2" s="3" t="inlineStr"/>
+      <c r="I2" s="3" t="inlineStr"/>
+      <c r="J2" s="3" t="inlineStr"/>
       <c r="K2" s="3" t="n"/>
       <c r="L2" s="3" t="n"/>
       <c r="M2" s="3" t="n"/>
@@ -781,39 +757,15 @@
           <t>A1</t>
         </is>
       </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>A45</t>
-        </is>
-      </c>
-      <c r="C3" s="3" t="inlineStr">
-        <is>
-          <t>A5</t>
-        </is>
-      </c>
-      <c r="D3" s="3" t="inlineStr">
-        <is>
-          <t>A45</t>
-        </is>
-      </c>
-      <c r="E3" s="3" t="inlineStr">
-        <is>
-          <t>A23</t>
-        </is>
-      </c>
-      <c r="F3" s="3" t="inlineStr">
-        <is>
-          <t>A56</t>
-        </is>
-      </c>
-      <c r="G3" s="3" t="inlineStr">
-        <is>
-          <t>A234</t>
-        </is>
-      </c>
-      <c r="H3" s="3" t="n"/>
-      <c r="I3" s="3" t="n"/>
-      <c r="J3" s="3" t="n"/>
+      <c r="B3" s="3" t="inlineStr"/>
+      <c r="C3" s="3" t="inlineStr"/>
+      <c r="D3" s="3" t="inlineStr"/>
+      <c r="E3" s="3" t="inlineStr"/>
+      <c r="F3" s="3" t="inlineStr"/>
+      <c r="G3" s="3" t="inlineStr"/>
+      <c r="H3" s="3" t="inlineStr"/>
+      <c r="I3" s="3" t="inlineStr"/>
+      <c r="J3" s="3" t="inlineStr"/>
       <c r="K3" s="3" t="n"/>
       <c r="L3" s="3" t="n"/>
       <c r="M3" s="3" t="n"/>
@@ -856,17 +808,17 @@
       </c>
       <c r="H4" s="3" t="inlineStr">
         <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="I4" s="3" t="inlineStr">
+        <is>
           <t>USD</t>
         </is>
       </c>
-      <c r="I4" s="3" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
       <c r="J4" s="3" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>PLN</t>
         </is>
       </c>
       <c r="K4" s="3" t="inlineStr">

</xml_diff>

<commit_message>
code refactorisation and some patches
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -472,7 +472,7 @@
     <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>27647,71</t>
+          <t>27525,92</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
@@ -499,7 +499,7 @@
     <row r="2" ht="12.8" customHeight="1" s="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>64,65</t>
+          <t>0,5243</t>
         </is>
       </c>
     </row>
@@ -577,6 +577,13 @@
       <c r="A13" s="3" t="inlineStr">
         <is>
           <t>143,76</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="inlineStr">
+        <is>
+          <t>4,3709</t>
         </is>
       </c>
     </row>
@@ -673,12 +680,12 @@
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ethereum</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>usd</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
@@ -738,8 +745,16 @@
           <t>Sheet1</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr"/>
-      <c r="C2" s="3" t="inlineStr"/>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>Arkusz3</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>Sheet1</t>
+        </is>
+      </c>
       <c r="D2" s="3" t="inlineStr"/>
       <c r="E2" s="3" t="inlineStr"/>
       <c r="F2" s="3" t="inlineStr"/>
@@ -754,11 +769,19 @@
     <row r="3" ht="15" customHeight="1" s="2">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>A1</t>
-        </is>
-      </c>
-      <c r="B3" s="3" t="inlineStr"/>
-      <c r="C3" s="3" t="inlineStr"/>
+          <t>A34</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>A56</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>A23</t>
+        </is>
+      </c>
       <c r="D3" s="3" t="inlineStr"/>
       <c r="E3" s="3" t="inlineStr"/>
       <c r="F3" s="3" t="inlineStr"/>
@@ -778,12 +801,12 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>EUR</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>GBP</t>
+          <t>PLN</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">

</xml_diff>

<commit_message>
autosuggtext repaired, scripts added, mypy update
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -569,7 +569,7 @@
     <row r="12" ht="12.8" customHeight="1" s="2">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>64,28</t>
+          <t>27831,72</t>
         </is>
       </c>
     </row>
@@ -584,6 +584,13 @@
       <c r="A23" s="3" t="inlineStr">
         <is>
           <t>4,3585</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="3" t="inlineStr">
+        <is>
+          <t>64,77</t>
         </is>
       </c>
     </row>
@@ -682,17 +689,17 @@
     <row r="1" ht="15" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>bitcoin</t>
+          <t>ethereum</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>ethereum</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>usd</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
@@ -749,19 +756,11 @@
     <row r="2" ht="12.8" customHeight="1" s="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>Sheet1</t>
-        </is>
-      </c>
-      <c r="B2" s="3" t="inlineStr">
-        <is>
           <t>Arkusz3</t>
         </is>
       </c>
-      <c r="C2" s="3" t="inlineStr">
-        <is>
-          <t>Sheet1</t>
-        </is>
-      </c>
+      <c r="B2" s="3" t="inlineStr"/>
+      <c r="C2" s="3" t="inlineStr"/>
       <c r="D2" s="3" t="inlineStr"/>
       <c r="E2" s="3" t="inlineStr"/>
       <c r="F2" s="3" t="inlineStr"/>
@@ -779,16 +778,8 @@
           <t>A1</t>
         </is>
       </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>A65</t>
-        </is>
-      </c>
-      <c r="C3" s="3" t="inlineStr">
-        <is>
-          <t>A5</t>
-        </is>
-      </c>
+      <c r="B3" s="3" t="inlineStr"/>
+      <c r="C3" s="3" t="inlineStr"/>
       <c r="D3" s="3" t="inlineStr"/>
       <c r="E3" s="3" t="inlineStr"/>
       <c r="F3" s="3" t="inlineStr"/>
@@ -906,14 +897,14 @@
     <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>1887,36</t>
+          <t>1619,25</t>
         </is>
       </c>
     </row>
     <row r="2" ht="12.8" customHeight="1" s="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>4,3943</t>
+          <t>27917,81</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add button changed, coloring name of error asset, fix change asset check input
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -472,7 +472,7 @@
     <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>27604,91</t>
+          <t>27597,38</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
@@ -583,7 +583,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>1583,91</t>
+          <t>1585,08</t>
         </is>
       </c>
     </row>
@@ -685,7 +685,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>

</xml_diff>

<commit_message>
info about succes or failed data saving
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -472,7 +472,7 @@
     <row r="1" ht="12.8" customHeight="1" s="2">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>27597,38</t>
+          <t>27372,29</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
@@ -513,7 +513,7 @@
     <row r="4" ht="12.8" customHeight="1" s="2">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>1,216</t>
+          <t>4,2809</t>
         </is>
       </c>
     </row>
@@ -583,7 +583,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>1585,08</t>
+          <t>1559,83</t>
         </is>
       </c>
     </row>
@@ -706,7 +706,7 @@
       </c>
       <c r="C1" s="3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>usd</t>
         </is>
       </c>
       <c r="D1" s="3" t="inlineStr">
@@ -771,7 +771,11 @@
           <t>Sheet1</t>
         </is>
       </c>
-      <c r="C2" s="3" t="inlineStr"/>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>Sheet1</t>
+        </is>
+      </c>
       <c r="D2" s="3" t="inlineStr"/>
       <c r="E2" s="3" t="inlineStr"/>
       <c r="F2" s="3" t="inlineStr"/>
@@ -794,7 +798,11 @@
           <t>A23</t>
         </is>
       </c>
-      <c r="C3" s="3" t="inlineStr"/>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>A4</t>
+        </is>
+      </c>
       <c r="D3" s="3" t="inlineStr"/>
       <c r="E3" s="3" t="inlineStr"/>
       <c r="F3" s="3" t="inlineStr"/>
@@ -819,7 +827,7 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>PLN</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">

</xml_diff>